<commit_message>
updated tests to increase code coverage
</commit_message>
<xml_diff>
--- a/griffinApp/griffinApp-JarModule/src/test/resources/failureClassService/validData.xlsx
+++ b/griffinApp/griffinApp-JarModule/src/test/resources/failureClassService/validData.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilmirnicanor/Desktop/College/continuous-build/griffinApp/griffinApp-JarModule/src/test/resources/importData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6010C817-FADC-444A-9E74-E70B0629B236}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D3B7AE15-7414-4E1F-BE74-BBC491B1DBF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="24240" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="23304" windowHeight="13224" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Data" sheetId="1" r:id="rId1"/>
@@ -22,7 +17,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Base Data'!$A$1:$N$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A88:C93"/>
 </workbook>
 </file>
 
@@ -1412,27 +1408,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="20.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1640625" style="6"/>
+    <col min="15" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1476,7 +1472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>43841.71875</v>
       </c>
@@ -1520,7 +1516,7 @@
         <v>1.1504449409094799E+18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>43841.71875</v>
       </c>
@@ -1564,7 +1560,7 @@
         <v>1.1504449409094799E+18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>43841.71875</v>
       </c>
@@ -1608,7 +1604,7 @@
         <v>1.1504449409094799E+18</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>43841.71875</v>
       </c>
@@ -1674,15 +1670,15 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="256" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="85.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="256" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1693,7 +1689,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1704,7 +1700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1715,7 +1711,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1726,7 +1722,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1737,7 +1733,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1748,7 +1744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1759,7 +1755,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1770,7 +1766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1781,7 +1777,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1792,7 +1788,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1803,7 +1799,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1814,7 +1810,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1825,7 +1821,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1836,7 +1832,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1847,7 +1843,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1858,7 +1854,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1869,7 +1865,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1880,7 +1876,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -1891,7 +1887,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1902,7 +1898,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1913,7 +1909,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1924,7 +1920,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -1935,7 +1931,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1946,7 +1942,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1957,7 +1953,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1968,7 +1964,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4</v>
       </c>
@@ -1979,7 +1975,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>5</v>
       </c>
@@ -1990,7 +1986,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>6</v>
       </c>
@@ -2001,7 +1997,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>7</v>
       </c>
@@ -2012,7 +2008,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>8</v>
       </c>
@@ -2023,7 +2019,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>9</v>
       </c>
@@ -2034,7 +2030,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>10</v>
       </c>
@@ -2045,7 +2041,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>11</v>
       </c>
@@ -2056,7 +2052,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>12</v>
       </c>
@@ -2067,7 +2063,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>13</v>
       </c>
@@ -2078,7 +2074,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>14</v>
       </c>
@@ -2089,7 +2085,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>15</v>
       </c>
@@ -2100,7 +2096,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>16</v>
       </c>
@@ -2111,7 +2107,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>17</v>
       </c>
@@ -2122,7 +2118,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>18</v>
       </c>
@@ -2133,7 +2129,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>19</v>
       </c>
@@ -2144,7 +2140,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>20</v>
       </c>
@@ -2155,7 +2151,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>21</v>
       </c>
@@ -2166,7 +2162,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>22</v>
       </c>
@@ -2177,7 +2173,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>23</v>
       </c>
@@ -2188,7 +2184,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>24</v>
       </c>
@@ -2199,7 +2195,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>25</v>
       </c>
@@ -2210,7 +2206,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>26</v>
       </c>
@@ -2221,7 +2217,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>27</v>
       </c>
@@ -2232,7 +2228,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>28</v>
       </c>
@@ -2243,7 +2239,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>29</v>
       </c>
@@ -2254,7 +2250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>30</v>
       </c>
@@ -2265,7 +2261,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>31</v>
       </c>
@@ -2276,7 +2272,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>32</v>
       </c>
@@ -2287,7 +2283,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>33</v>
       </c>
@@ -2298,7 +2294,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>0</v>
       </c>
@@ -2309,7 +2305,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1</v>
       </c>
@@ -2320,7 +2316,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2</v>
       </c>
@@ -2331,7 +2327,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>3</v>
       </c>
@@ -2342,7 +2338,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>4</v>
       </c>
@@ -2353,7 +2349,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>5</v>
       </c>
@@ -2364,7 +2360,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>6</v>
       </c>
@@ -2375,7 +2371,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>7</v>
       </c>
@@ -2386,7 +2382,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>8</v>
       </c>
@@ -2397,7 +2393,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>9</v>
       </c>
@@ -2408,7 +2404,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>10</v>
       </c>
@@ -2419,7 +2415,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>11</v>
       </c>
@@ -2430,7 +2426,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>12</v>
       </c>
@@ -2441,7 +2437,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>13</v>
       </c>
@@ -2452,7 +2448,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>14</v>
       </c>
@@ -2463,7 +2459,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>15</v>
       </c>
@@ -2474,7 +2470,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>16</v>
       </c>
@@ -2485,7 +2481,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>17</v>
       </c>
@@ -2496,7 +2492,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>18</v>
       </c>
@@ -2507,7 +2503,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>19</v>
       </c>
@@ -2518,7 +2514,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>20</v>
       </c>
@@ -2529,7 +2525,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>21</v>
       </c>
@@ -2540,7 +2536,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>22</v>
       </c>
@@ -2551,7 +2547,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>23</v>
       </c>
@@ -2562,7 +2558,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>24</v>
       </c>
@@ -2594,16 +2590,16 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="85.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="256" width="8.83203125" customWidth="1"/>
+    <col min="2" max="2" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="85.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="256" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>97</v>
       </c>
@@ -2611,7 +2607,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -2619,7 +2615,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -2627,7 +2623,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -2635,7 +2631,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -2643,7 +2639,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -2668,25 +2664,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
     <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="4" width="255.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5" customWidth="1"/>
-    <col min="6" max="6" width="41.5" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" customWidth="1"/>
+    <col min="6" max="6" width="41.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="256" width="8.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="256" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2715,7 +2711,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>100100</v>
       </c>
@@ -2744,7 +2740,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>100200</v>
       </c>
@@ -2773,7 +2769,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>100300</v>
       </c>
@@ -2802,7 +2798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>100400</v>
       </c>
@@ -2831,7 +2827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>100500</v>
       </c>
@@ -2860,7 +2856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>100600</v>
       </c>
@@ -2889,7 +2885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>100700</v>
       </c>
@@ -2918,7 +2914,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>100800</v>
       </c>
@@ -2947,7 +2943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>100900</v>
       </c>
@@ -2976,7 +2972,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>101000</v>
       </c>
@@ -3005,7 +3001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>101300</v>
       </c>
@@ -3034,7 +3030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>101500</v>
       </c>
@@ -3063,7 +3059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>101600</v>
       </c>
@@ -3092,7 +3088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>101700</v>
       </c>
@@ -3121,7 +3117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>101710</v>
       </c>
@@ -3150,7 +3146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>101800</v>
       </c>
@@ -3179,7 +3175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>102000</v>
       </c>
@@ -3208,7 +3204,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>102100</v>
       </c>
@@ -3237,7 +3233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>102200</v>
       </c>
@@ -3266,7 +3262,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>102300</v>
       </c>
@@ -3295,7 +3291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>102400</v>
       </c>
@@ -3324,7 +3320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>102500</v>
       </c>
@@ -3353,7 +3349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>102600</v>
       </c>
@@ -3382,7 +3378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>102700</v>
       </c>
@@ -3411,7 +3407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>102800</v>
       </c>
@@ -3440,7 +3436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>102900</v>
       </c>
@@ -3469,7 +3465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>103000</v>
       </c>
@@ -3498,7 +3494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>103100</v>
       </c>
@@ -3527,7 +3523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>103200</v>
       </c>
@@ -3556,7 +3552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>103300</v>
       </c>
@@ -3585,7 +3581,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>103500</v>
       </c>
@@ -3614,7 +3610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>103600</v>
       </c>
@@ -3643,7 +3639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>103700</v>
       </c>
@@ -3672,7 +3668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>103800</v>
       </c>
@@ -3701,7 +3697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>103900</v>
       </c>
@@ -3730,7 +3726,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>104100</v>
       </c>
@@ -3759,7 +3755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>104200</v>
       </c>
@@ -3788,7 +3784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>104400</v>
       </c>
@@ -3817,7 +3813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>104500</v>
       </c>
@@ -3846,7 +3842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>104600</v>
       </c>
@@ -3875,7 +3871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>104700</v>
       </c>
@@ -3904,7 +3900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>104800</v>
       </c>
@@ -3933,7 +3929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>105000</v>
       </c>
@@ -3962,7 +3958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>105200</v>
       </c>
@@ -3991,7 +3987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>105300</v>
       </c>
@@ -4020,7 +4016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>105400</v>
       </c>
@@ -4049,7 +4045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>105500</v>
       </c>
@@ -4078,7 +4074,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>105600</v>
       </c>
@@ -4107,7 +4103,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>105700</v>
       </c>
@@ -4136,7 +4132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>105900</v>
       </c>
@@ -4165,7 +4161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>106200</v>
       </c>
@@ -4194,7 +4190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>106400</v>
       </c>
@@ -4223,7 +4219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>106500</v>
       </c>
@@ -4252,7 +4248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>106600</v>
       </c>
@@ -4281,7 +4277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>106700</v>
       </c>
@@ -4310,7 +4306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>106900</v>
       </c>
@@ -4339,7 +4335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>107100</v>
       </c>
@@ -4368,7 +4364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>107200</v>
       </c>
@@ -4397,7 +4393,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>107400</v>
       </c>
@@ -4426,7 +4422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>107600</v>
       </c>
@@ -4455,7 +4451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>107700</v>
       </c>
@@ -4484,7 +4480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>107800</v>
       </c>
@@ -4513,7 +4509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>107900</v>
       </c>
@@ -4542,7 +4538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>108000</v>
       </c>
@@ -4571,7 +4567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>108100</v>
       </c>
@@ -4600,7 +4596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>108200</v>
       </c>
@@ -4629,7 +4625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>108300</v>
       </c>
@@ -4658,7 +4654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>108400</v>
       </c>
@@ -4687,7 +4683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>116000</v>
       </c>
@@ -4716,7 +4712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>21060800</v>
       </c>
@@ -4745,7 +4741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>33000153</v>
       </c>
@@ -4774,7 +4770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>33000253</v>
       </c>
@@ -4803,7 +4799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>33000353</v>
       </c>
@@ -4832,7 +4828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <v>33000453</v>
       </c>
@@ -4861,7 +4857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
         <v>33000553</v>
       </c>
@@ -4890,7 +4886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
         <v>33000635</v>
       </c>
@@ -4919,7 +4915,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="6">
         <v>33000753</v>
       </c>
@@ -4948,7 +4944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="6">
         <v>33000853</v>
       </c>
@@ -4977,7 +4973,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="6">
         <v>33000953</v>
       </c>
@@ -5006,7 +5002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="6">
         <v>33001053</v>
       </c>
@@ -5035,7 +5031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="6">
         <v>33001195</v>
       </c>
@@ -5064,7 +5060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="6">
         <v>33001235</v>
       </c>
@@ -5093,7 +5089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="6">
         <v>33001295</v>
       </c>
@@ -5122,7 +5118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="6">
         <v>33001453</v>
       </c>
@@ -5151,7 +5147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="6">
         <v>33001553</v>
       </c>
@@ -5180,7 +5176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="6">
         <v>33001635</v>
       </c>
@@ -5209,7 +5205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="6">
         <v>33001695</v>
       </c>
@@ -5238,7 +5234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="6">
         <v>33001735</v>
       </c>
@@ -5267,7 +5263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="6">
         <v>33001835</v>
       </c>
@@ -5296,7 +5292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
         <v>33001953</v>
       </c>
@@ -5325,7 +5321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="6">
         <v>33002053</v>
       </c>
@@ -5354,7 +5350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
         <v>33002135</v>
       </c>
@@ -5383,7 +5379,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="6">
         <v>33002195</v>
       </c>
@@ -5412,7 +5408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="6">
         <v>33002235</v>
       </c>
@@ -5441,7 +5437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="6">
         <v>33002295</v>
       </c>
@@ -5470,7 +5466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="6">
         <v>33002353</v>
       </c>
@@ -5499,7 +5495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="6">
         <v>33002499</v>
       </c>
@@ -5528,7 +5524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="6">
         <v>33002535</v>
       </c>
@@ -5557,7 +5553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="6">
         <v>33002635</v>
       </c>
@@ -5599,12 +5595,12 @@
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="256" width="8.83203125" customWidth="1"/>
+    <col min="1" max="256" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>295</v>
       </c>
@@ -5618,7 +5614,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>238</v>
       </c>
@@ -5632,7 +5628,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>238</v>
       </c>
@@ -5646,7 +5642,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>238</v>
       </c>
@@ -5660,7 +5656,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>240</v>
       </c>
@@ -5674,7 +5670,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>240</v>
       </c>
@@ -5688,7 +5684,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>240</v>
       </c>
@@ -5702,7 +5698,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>240</v>
       </c>
@@ -5716,7 +5712,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>240</v>
       </c>
@@ -5730,7 +5726,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>302</v>
       </c>
@@ -5744,7 +5740,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>302</v>
       </c>
@@ -5758,7 +5754,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>302</v>
       </c>
@@ -5772,7 +5768,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>302</v>
       </c>
@@ -5786,7 +5782,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>310</v>
       </c>
@@ -5800,7 +5796,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>310</v>
       </c>
@@ -5814,7 +5810,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>310</v>
       </c>
@@ -5828,7 +5824,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>310</v>
       </c>
@@ -5842,7 +5838,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>310</v>
       </c>
@@ -5856,7 +5852,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>310</v>
       </c>
@@ -5870,7 +5866,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>310</v>
       </c>
@@ -5884,7 +5880,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>310</v>
       </c>
@@ -5898,7 +5894,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>310</v>
       </c>
@@ -5912,7 +5908,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>340</v>
       </c>
@@ -5926,7 +5922,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>340</v>
       </c>
@@ -5940,7 +5936,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>340</v>
       </c>
@@ -5954,7 +5950,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>344</v>
       </c>
@@ -5968,7 +5964,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>344</v>
       </c>
@@ -5982,7 +5978,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>344</v>
       </c>
@@ -5996,7 +5992,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>405</v>
       </c>
@@ -6010,7 +6006,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>405</v>
       </c>
@@ -6024,7 +6020,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>405</v>
       </c>
@@ -6038,7 +6034,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>405</v>
       </c>
@@ -6052,7 +6048,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>405</v>
       </c>
@@ -6066,7 +6062,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>440</v>
       </c>
@@ -6080,7 +6076,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>440</v>
       </c>
@@ -6094,7 +6090,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>440</v>
       </c>
@@ -6108,7 +6104,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>505</v>
       </c>
@@ -6122,7 +6118,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>505</v>
       </c>
@@ -6136,7 +6132,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>505</v>
       </c>
@@ -6150,7 +6146,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>505</v>
       </c>
@@ -6164,7 +6160,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>505</v>
       </c>
@@ -6178,7 +6174,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>505</v>
       </c>

</xml_diff>